<commit_message>
Today i have started week5 with insertion sort
</commit_message>
<xml_diff>
--- a/Coder Army Sheet (1).xlsx
+++ b/Coder Army Sheet (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Coder Army\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834BB857-0689-40B0-B5BB-DF7498597D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB9422D-8302-4ED4-A0A7-46461DF0C134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2979,8 +2979,8 @@
   </sheetPr>
   <dimension ref="A1:E746"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4492,7 +4492,7 @@
         <v>29</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>11</v>
+        <v>751</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -4509,7 +4509,7 @@
         <v>29</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>11</v>
+        <v>751</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -4526,7 +4526,7 @@
         <v>29</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>11</v>
+        <v>751</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -4543,7 +4543,7 @@
         <v>29</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>11</v>
+        <v>751</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -4560,7 +4560,7 @@
         <v>30</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>11</v>
+        <v>751</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -4594,7 +4594,7 @@
         <v>30</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>11</v>
+        <v>751</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -4611,7 +4611,7 @@
         <v>30</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>11</v>
+        <v>751</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -4645,7 +4645,7 @@
         <v>31</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>11</v>
+        <v>751</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -4696,7 +4696,7 @@
         <v>32</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>11</v>
+        <v>751</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
today i am solving the problem based  on binary search
</commit_message>
<xml_diff>
--- a/Coder Army Sheet (1).xlsx
+++ b/Coder Army Sheet (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Coder Army\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB9422D-8302-4ED4-A0A7-46461DF0C134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75E66A8-D372-4C99-86D1-40E51EAF7D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2980,7 +2980,7 @@
   <dimension ref="A1:E746"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Today i am learn and implement floyd warshlle algorithm
</commit_message>
<xml_diff>
--- a/Coder Army Sheet (1).xlsx
+++ b/Coder Army Sheet (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Coder Army\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ECE8E0-3DF8-4C08-A297-F5506C480C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7F5C80-E6B2-4CF6-B406-A9AE2E2699A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2926" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2930" uniqueCount="753">
   <si>
     <t>Hard work Beats Talent When Talent Doesn't work Hard</t>
   </si>
@@ -2991,8 +2991,8 @@
   </sheetPr>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G27" activeCellId="1" sqref="E22:F22 G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3341,8 +3341,11 @@
       <c r="D19" s="7">
         <v>4</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>11</v>
+      <c r="E19" s="36" t="s">
+        <v>751</v>
+      </c>
+      <c r="F19" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3358,8 +3361,11 @@
       <c r="D20" s="7">
         <v>4</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>11</v>
+      <c r="E20" s="36" t="s">
+        <v>751</v>
+      </c>
+      <c r="F20" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3375,8 +3381,11 @@
       <c r="D21" s="7">
         <v>5</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>11</v>
+      <c r="E21" s="36" t="s">
+        <v>751</v>
+      </c>
+      <c r="F21" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3392,8 +3401,11 @@
       <c r="D22" s="7">
         <v>5</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>11</v>
+      <c r="E22" s="36" t="s">
+        <v>751</v>
+      </c>
+      <c r="F22" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Today i am learn about Eulier Path and Eulier circuit
</commit_message>
<xml_diff>
--- a/Coder Army Sheet (1).xlsx
+++ b/Coder Army Sheet (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Coder Army\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7F5C80-E6B2-4CF6-B406-A9AE2E2699A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B027F4-3484-4AF4-A04E-CAD5CF42D2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2930" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2932" uniqueCount="753">
   <si>
     <t>Hard work Beats Talent When Talent Doesn't work Hard</t>
   </si>
@@ -2992,7 +2992,7 @@
   <dimension ref="A1:F746"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G27" activeCellId="1" sqref="E22:F22 G27"/>
+      <selection activeCell="E27" activeCellId="1" sqref="E24:F24 E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3421,8 +3421,11 @@
       <c r="D23" s="7">
         <v>5</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>11</v>
+      <c r="E23" s="36" t="s">
+        <v>751</v>
+      </c>
+      <c r="F23" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3438,8 +3441,11 @@
       <c r="D24" s="7">
         <v>5</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>11</v>
+      <c r="E24" s="36" t="s">
+        <v>751</v>
+      </c>
+      <c r="F24" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
solve the particular problems in one go
</commit_message>
<xml_diff>
--- a/Coder Army Sheet (1).xlsx
+++ b/Coder Army Sheet (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Coder Army\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B027F4-3484-4AF4-A04E-CAD5CF42D2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EFB873-4C5F-483A-8B6F-5281ACBDD51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2991,8 +2991,8 @@
   </sheetPr>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E27" activeCellId="1" sqref="E24:F24 E27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3890,7 +3890,7 @@
       <c r="C51" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="36">
         <v>15</v>
       </c>
       <c r="E51" s="7" t="s">
@@ -3907,7 +3907,7 @@
       <c r="C52" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="36">
         <v>15</v>
       </c>
       <c r="E52" s="7" t="s">
@@ -3924,7 +3924,7 @@
       <c r="C53" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="36">
         <v>15</v>
       </c>
       <c r="E53" s="7" t="s">
@@ -3941,7 +3941,7 @@
       <c r="C54" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D54" s="36">
         <v>15</v>
       </c>
       <c r="E54" s="7" t="s">
@@ -3992,7 +3992,7 @@
       <c r="C57" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="36">
         <v>16</v>
       </c>
       <c r="E57" s="7" t="s">

</xml_diff>